<commit_message>
update kode kertas senavbah 2021
</commit_message>
<xml_diff>
--- a/21. SENAVBAH 2021/SENAVBAH 2021.xlsx
+++ b/21. SENAVBAH 2021/SENAVBAH 2021.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\21. SENAVBAH 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{546C8D62-C02E-49DE-8516-5593E2567787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791CF40B-1E2D-4FF3-A0BE-7DF958819469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="CETAK " sheetId="2" r:id="rId2"/>
+    <sheet name="REKAP" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'CETAK '!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="363">
   <si>
     <t>NO</t>
   </si>
@@ -1040,11 +1041,101 @@
   <si>
     <t>FAHRI</t>
   </si>
+  <si>
+    <t>KELAS</t>
+  </si>
+  <si>
+    <t>KODE</t>
+  </si>
+  <si>
+    <t>JUMLAH</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-1 NAV "B"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-1 NAV "A"</t>
+  </si>
+  <si>
+    <t>DIKMATA XL-2 NAV "B"</t>
+  </si>
+  <si>
+    <t>DIKMATA XL-2 NAV "A"</t>
+  </si>
+  <si>
+    <t>DIKMATA XL-2 BAH "A"</t>
+  </si>
+  <si>
+    <t>DIKMATA XL-2 BAH "B"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-1 BAH "A"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-2 BAH "A"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-2 BAH "B"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-1 BAH "B"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-2 NAV "A"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-2 NAV "B"</t>
+  </si>
+  <si>
+    <t>DIKMABA XL-2 NAV "C"</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>KERTAS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1160,7 +1251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1258,6 +1349,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1629,10 +1721,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y425"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:F271"/>
     </sheetView>
@@ -1654,20 +1746,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="13" t="s">
@@ -1793,7 +1885,7 @@
         <v>99</v>
       </c>
       <c r="X2" s="21">
-        <f>COUNTIF($C$2:$C$271,C2)</f>
+        <f t="shared" ref="X2:X65" si="0">COUNTIF($C$2:$C$271,C2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1865,7 +1957,7 @@
         <v>100</v>
       </c>
       <c r="X3" s="21">
-        <f>COUNTIF($C$2:$C$271,C3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1937,7 +2029,7 @@
         <v>100</v>
       </c>
       <c r="X4" s="21">
-        <f>COUNTIF($C$2:$C$271,C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2009,7 +2101,7 @@
         <v>104</v>
       </c>
       <c r="X5" s="21">
-        <f>COUNTIF($C$2:$C$271,C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2081,7 +2173,7 @@
         <v>100</v>
       </c>
       <c r="X6" s="21">
-        <f>COUNTIF($C$2:$C$271,C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2153,7 +2245,7 @@
         <v>105</v>
       </c>
       <c r="X7" s="21">
-        <f>COUNTIF($C$2:$C$271,C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2225,7 +2317,7 @@
         <v>103</v>
       </c>
       <c r="X8" s="21">
-        <f>COUNTIF($C$2:$C$271,C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2297,7 +2389,7 @@
         <v>104</v>
       </c>
       <c r="X9" s="21">
-        <f>COUNTIF($C$2:$C$271,C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2369,7 +2461,7 @@
         <v>102</v>
       </c>
       <c r="X10" s="21">
-        <f>COUNTIF($C$2:$C$271,C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2441,7 +2533,7 @@
         <v>108</v>
       </c>
       <c r="X11" s="21">
-        <f>COUNTIF($C$2:$C$271,C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2513,7 +2605,7 @@
         <v>100</v>
       </c>
       <c r="X12" s="21">
-        <f>COUNTIF($C$2:$C$271,C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2585,7 +2677,7 @@
         <v>102</v>
       </c>
       <c r="X13" s="21">
-        <f>COUNTIF($C$2:$C$271,C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2657,7 +2749,7 @@
         <v>100</v>
       </c>
       <c r="X14" s="21">
-        <f>COUNTIF($C$2:$C$271,C14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2729,7 +2821,7 @@
         <v>105</v>
       </c>
       <c r="X15" s="21">
-        <f>COUNTIF($C$2:$C$271,C15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2801,7 +2893,7 @@
         <v>105</v>
       </c>
       <c r="X16" s="21">
-        <f>COUNTIF($C$2:$C$271,C16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2873,7 +2965,7 @@
         <v>109</v>
       </c>
       <c r="X17" s="21">
-        <f>COUNTIF($C$2:$C$271,C17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2945,7 +3037,7 @@
         <v>102</v>
       </c>
       <c r="X18" s="21">
-        <f>COUNTIF($C$2:$C$271,C18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3017,7 +3109,7 @@
         <v>101</v>
       </c>
       <c r="X19" s="21">
-        <f>COUNTIF($C$2:$C$271,C19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3089,7 +3181,7 @@
         <v>101</v>
       </c>
       <c r="X20" s="21">
-        <f>COUNTIF($C$2:$C$271,C20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3161,7 +3253,7 @@
         <v>102</v>
       </c>
       <c r="X21" s="21">
-        <f>COUNTIF($C$2:$C$271,C21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3233,7 +3325,7 @@
         <v>104</v>
       </c>
       <c r="X22" s="21">
-        <f>COUNTIF($C$2:$C$271,C22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3305,7 +3397,7 @@
         <v>103</v>
       </c>
       <c r="X23" s="21">
-        <f>COUNTIF($C$2:$C$271,C23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3377,7 +3469,7 @@
         <v>105</v>
       </c>
       <c r="X24" s="21">
-        <f>COUNTIF($C$2:$C$271,C24)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3449,7 +3541,7 @@
         <v>100</v>
       </c>
       <c r="X25" s="21">
-        <f>COUNTIF($C$2:$C$271,C25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3521,7 +3613,7 @@
         <v>99</v>
       </c>
       <c r="X26" s="21">
-        <f>COUNTIF($C$2:$C$271,C26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3593,7 +3685,7 @@
         <v>106</v>
       </c>
       <c r="X27" s="21">
-        <f>COUNTIF($C$2:$C$271,C27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3665,7 +3757,7 @@
         <v>101</v>
       </c>
       <c r="X28" s="21">
-        <f>COUNTIF($C$2:$C$271,C28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3737,7 +3829,7 @@
         <v>100</v>
       </c>
       <c r="X29" s="21">
-        <f>COUNTIF($C$2:$C$271,C29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3809,7 +3901,7 @@
         <v>108</v>
       </c>
       <c r="X30" s="21">
-        <f>COUNTIF($C$2:$C$271,C30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3881,7 +3973,7 @@
         <v>102</v>
       </c>
       <c r="X31" s="21">
-        <f>COUNTIF($C$2:$C$271,C31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3953,7 +4045,7 @@
         <v>99</v>
       </c>
       <c r="X32" s="21">
-        <f>COUNTIF($C$2:$C$271,C32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4025,7 +4117,7 @@
         <v>101</v>
       </c>
       <c r="X33" s="21">
-        <f>COUNTIF($C$2:$C$271,C33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4097,7 +4189,7 @@
         <v>100</v>
       </c>
       <c r="X34" s="21">
-        <f>COUNTIF($C$2:$C$271,C34)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4169,7 +4261,7 @@
         <v>100</v>
       </c>
       <c r="X35" s="21">
-        <f>COUNTIF($C$2:$C$271,C35)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4241,7 +4333,7 @@
         <v>110</v>
       </c>
       <c r="X36" s="21">
-        <f>COUNTIF($C$2:$C$271,C36)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4313,7 +4405,7 @@
         <v>99</v>
       </c>
       <c r="X37" s="21">
-        <f>COUNTIF($C$2:$C$271,C37)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4385,7 +4477,7 @@
         <v>108</v>
       </c>
       <c r="X38" s="21">
-        <f>COUNTIF($C$2:$C$271,C38)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4457,7 +4549,7 @@
         <v>98</v>
       </c>
       <c r="X39" s="21">
-        <f>COUNTIF($C$2:$C$271,C39)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4529,7 +4621,7 @@
         <v>103</v>
       </c>
       <c r="X40" s="21">
-        <f>COUNTIF($C$2:$C$271,C40)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4601,7 +4693,7 @@
         <v>98</v>
       </c>
       <c r="X41" s="21">
-        <f>COUNTIF($C$2:$C$271,C41)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4673,7 +4765,7 @@
         <v>107</v>
       </c>
       <c r="X42" s="21">
-        <f>COUNTIF($C$2:$C$271,C42)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4745,7 +4837,7 @@
         <v>100</v>
       </c>
       <c r="X43" s="21">
-        <f>COUNTIF($C$2:$C$271,C43)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4817,7 +4909,7 @@
         <v>103</v>
       </c>
       <c r="X44" s="21">
-        <f>COUNTIF($C$2:$C$271,C44)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4889,7 +4981,7 @@
         <v>102</v>
       </c>
       <c r="X45" s="21">
-        <f>COUNTIF($C$2:$C$271,C45)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4961,7 +5053,7 @@
         <v>101</v>
       </c>
       <c r="X46" s="21">
-        <f>COUNTIF($C$2:$C$271,C46)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5033,7 +5125,7 @@
         <v>103</v>
       </c>
       <c r="X47" s="21">
-        <f>COUNTIF($C$2:$C$271,C47)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5105,7 +5197,7 @@
         <v>102</v>
       </c>
       <c r="X48" s="21">
-        <f>COUNTIF($C$2:$C$271,C48)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5177,7 +5269,7 @@
         <v>100</v>
       </c>
       <c r="X49" s="21">
-        <f>COUNTIF($C$2:$C$271,C49)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5249,7 +5341,7 @@
         <v>108</v>
       </c>
       <c r="X50" s="21">
-        <f>COUNTIF($C$2:$C$271,C50)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -5321,7 +5413,7 @@
         <v>109</v>
       </c>
       <c r="X51" s="21">
-        <f>COUNTIF($C$2:$C$271,C51)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5393,7 +5485,7 @@
         <v>103</v>
       </c>
       <c r="X52" s="21">
-        <f>COUNTIF($C$2:$C$271,C52)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5465,7 +5557,7 @@
         <v>100</v>
       </c>
       <c r="X53" s="21">
-        <f>COUNTIF($C$2:$C$271,C53)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5537,7 +5629,7 @@
         <v>111</v>
       </c>
       <c r="X54" s="21">
-        <f>COUNTIF($C$2:$C$271,C54)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5609,7 +5701,7 @@
         <v>100</v>
       </c>
       <c r="X55" s="21">
-        <f>COUNTIF($C$2:$C$271,C55)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5681,7 +5773,7 @@
         <v>107</v>
       </c>
       <c r="X56" s="21">
-        <f>COUNTIF($C$2:$C$271,C56)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5753,7 +5845,7 @@
         <v>107</v>
       </c>
       <c r="X57" s="21">
-        <f>COUNTIF($C$2:$C$271,C57)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5825,7 +5917,7 @@
         <v>100</v>
       </c>
       <c r="X58" s="21">
-        <f>COUNTIF($C$2:$C$271,C58)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5897,7 +5989,7 @@
         <v>105</v>
       </c>
       <c r="X59" s="21">
-        <f>COUNTIF($C$2:$C$271,C59)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5969,7 +6061,7 @@
         <v>100</v>
       </c>
       <c r="X60" s="21">
-        <f>COUNTIF($C$2:$C$271,C60)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6041,7 +6133,7 @@
         <v>104</v>
       </c>
       <c r="X61" s="21">
-        <f>COUNTIF($C$2:$C$271,C61)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6113,7 +6205,7 @@
         <v>103</v>
       </c>
       <c r="X62" s="21">
-        <f>COUNTIF($C$2:$C$271,C62)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6185,7 +6277,7 @@
         <v>99</v>
       </c>
       <c r="X63" s="21">
-        <f>COUNTIF($C$2:$C$271,C63)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6257,7 +6349,7 @@
         <v>100</v>
       </c>
       <c r="X64" s="21">
-        <f>COUNTIF($C$2:$C$271,C64)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6329,7 +6421,7 @@
         <v>106</v>
       </c>
       <c r="X65" s="21">
-        <f>COUNTIF($C$2:$C$271,C65)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -6401,7 +6493,7 @@
         <v>98</v>
       </c>
       <c r="X66" s="21">
-        <f>COUNTIF($C$2:$C$271,C66)</f>
+        <f t="shared" ref="X66:X129" si="1">COUNTIF($C$2:$C$271,C66)</f>
         <v>1</v>
       </c>
     </row>
@@ -6473,7 +6565,7 @@
         <v>108</v>
       </c>
       <c r="X67" s="21">
-        <f>COUNTIF($C$2:$C$271,C67)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6545,7 +6637,7 @@
         <v>104</v>
       </c>
       <c r="X68" s="21">
-        <f>COUNTIF($C$2:$C$271,C68)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6617,7 +6709,7 @@
         <v>105</v>
       </c>
       <c r="X69" s="21">
-        <f>COUNTIF($C$2:$C$271,C69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6689,7 +6781,7 @@
         <v>108</v>
       </c>
       <c r="X70" s="21">
-        <f>COUNTIF($C$2:$C$271,C70)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6761,7 +6853,7 @@
         <v>106</v>
       </c>
       <c r="X71" s="21">
-        <f>COUNTIF($C$2:$C$271,C71)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6833,7 +6925,7 @@
         <v>98</v>
       </c>
       <c r="X72" s="21">
-        <f>COUNTIF($C$2:$C$271,C72)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6905,7 +6997,7 @@
         <v>105</v>
       </c>
       <c r="X73" s="21">
-        <f>COUNTIF($C$2:$C$271,C73)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6977,7 +7069,7 @@
         <v>101</v>
       </c>
       <c r="X74" s="21">
-        <f>COUNTIF($C$2:$C$271,C74)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7049,7 +7141,7 @@
         <v>99</v>
       </c>
       <c r="X75" s="21">
-        <f>COUNTIF($C$2:$C$271,C75)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7121,7 +7213,7 @@
         <v>103</v>
       </c>
       <c r="X76" s="21">
-        <f>COUNTIF($C$2:$C$271,C76)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7193,7 +7285,7 @@
         <v>105</v>
       </c>
       <c r="X77" s="21">
-        <f>COUNTIF($C$2:$C$271,C77)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7265,7 +7357,7 @@
         <v>101</v>
       </c>
       <c r="X78" s="21">
-        <f>COUNTIF($C$2:$C$271,C78)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7337,7 +7429,7 @@
         <v>100</v>
       </c>
       <c r="X79" s="21">
-        <f>COUNTIF($C$2:$C$271,C79)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7409,7 +7501,7 @@
         <v>100</v>
       </c>
       <c r="X80" s="21">
-        <f>COUNTIF($C$2:$C$271,C80)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7481,7 +7573,7 @@
         <v>101</v>
       </c>
       <c r="X81" s="21">
-        <f>COUNTIF($C$2:$C$271,C81)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7553,7 +7645,7 @@
         <v>100</v>
       </c>
       <c r="X82" s="21">
-        <f>COUNTIF($C$2:$C$271,C82)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7628,7 +7720,7 @@
         <v>330</v>
       </c>
       <c r="X83" s="21">
-        <f>COUNTIF($C$2:$C$271,C83)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7703,7 +7795,7 @@
         <v>331</v>
       </c>
       <c r="X84" s="21">
-        <f>COUNTIF($C$2:$C$271,C84)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7775,7 +7867,7 @@
         <v>101</v>
       </c>
       <c r="X85" s="21">
-        <f>COUNTIF($C$2:$C$271,C85)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7847,7 +7939,7 @@
         <v>100</v>
       </c>
       <c r="X86" s="21">
-        <f>COUNTIF($C$2:$C$271,C86)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7919,7 +8011,7 @@
         <v>102</v>
       </c>
       <c r="X87" s="21">
-        <f>COUNTIF($C$2:$C$271,C87)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7991,7 +8083,7 @@
         <v>97</v>
       </c>
       <c r="X88" s="21">
-        <f>COUNTIF($C$2:$C$271,C88)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8063,7 +8155,7 @@
         <v>100</v>
       </c>
       <c r="X89" s="21">
-        <f>COUNTIF($C$2:$C$271,C89)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8135,7 +8227,7 @@
         <v>104</v>
       </c>
       <c r="X90" s="21">
-        <f>COUNTIF($C$2:$C$271,C90)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8207,7 +8299,7 @@
         <v>101</v>
       </c>
       <c r="X91" s="21">
-        <f>COUNTIF($C$2:$C$271,C91)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8279,7 +8371,7 @@
         <v>100</v>
       </c>
       <c r="X92" s="21">
-        <f>COUNTIF($C$2:$C$271,C92)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8351,7 +8443,7 @@
         <v>102</v>
       </c>
       <c r="X93" s="21">
-        <f>COUNTIF($C$2:$C$271,C93)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8423,7 +8515,7 @@
         <v>101</v>
       </c>
       <c r="X94" s="21">
-        <f>COUNTIF($C$2:$C$271,C94)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8495,7 +8587,7 @@
         <v>100</v>
       </c>
       <c r="X95" s="21">
-        <f>COUNTIF($C$2:$C$271,C95)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8567,7 +8659,7 @@
         <v>103</v>
       </c>
       <c r="X96" s="21">
-        <f>COUNTIF($C$2:$C$271,C96)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8639,7 +8731,7 @@
         <v>101</v>
       </c>
       <c r="X97" s="21">
-        <f>COUNTIF($C$2:$C$271,C97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8711,7 +8803,7 @@
         <v>102</v>
       </c>
       <c r="X98" s="21">
-        <f>COUNTIF($C$2:$C$271,C98)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8783,7 +8875,7 @@
         <v>101</v>
       </c>
       <c r="X99" s="21">
-        <f>COUNTIF($C$2:$C$271,C99)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8855,7 +8947,7 @@
         <v>100</v>
       </c>
       <c r="X100" s="21">
-        <f>COUNTIF($C$2:$C$271,C100)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8927,7 +9019,7 @@
         <v>100</v>
       </c>
       <c r="X101" s="21">
-        <f>COUNTIF($C$2:$C$271,C101)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8999,7 +9091,7 @@
         <v>104</v>
       </c>
       <c r="X102" s="21">
-        <f>COUNTIF($C$2:$C$271,C102)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9071,7 +9163,7 @@
         <v>101</v>
       </c>
       <c r="X103" s="21">
-        <f>COUNTIF($C$2:$C$271,C103)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9143,7 +9235,7 @@
         <v>99</v>
       </c>
       <c r="X104" s="21">
-        <f>COUNTIF($C$2:$C$271,C104)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9215,7 +9307,7 @@
         <v>101</v>
       </c>
       <c r="X105" s="21">
-        <f>COUNTIF($C$2:$C$271,C105)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9287,7 +9379,7 @@
         <v>101</v>
       </c>
       <c r="X106" s="21">
-        <f>COUNTIF($C$2:$C$271,C106)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9359,7 +9451,7 @@
         <v>96</v>
       </c>
       <c r="X107" s="21">
-        <f>COUNTIF($C$2:$C$271,C107)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9431,7 +9523,7 @@
         <v>97</v>
       </c>
       <c r="X108" s="21">
-        <f>COUNTIF($C$2:$C$271,C108)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9503,7 +9595,7 @@
         <v>98</v>
       </c>
       <c r="X109" s="21">
-        <f>COUNTIF($C$2:$C$271,C109)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9575,7 +9667,7 @@
         <v>100</v>
       </c>
       <c r="X110" s="21">
-        <f>COUNTIF($C$2:$C$271,C110)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9647,7 +9739,7 @@
         <v>98</v>
       </c>
       <c r="X111" s="21">
-        <f>COUNTIF($C$2:$C$271,C111)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9719,7 +9811,7 @@
         <v>103</v>
       </c>
       <c r="X112" s="21">
-        <f>COUNTIF($C$2:$C$271,C112)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9791,7 +9883,7 @@
         <v>98</v>
       </c>
       <c r="X113" s="21">
-        <f>COUNTIF($C$2:$C$271,C113)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9863,7 +9955,7 @@
         <v>97</v>
       </c>
       <c r="X114" s="21">
-        <f>COUNTIF($C$2:$C$271,C114)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -9935,7 +10027,7 @@
         <v>100</v>
       </c>
       <c r="X115" s="21">
-        <f>COUNTIF($C$2:$C$271,C115)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10007,7 +10099,7 @@
         <v>97</v>
       </c>
       <c r="X116" s="21">
-        <f>COUNTIF($C$2:$C$271,C116)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10079,7 +10171,7 @@
         <v>102</v>
       </c>
       <c r="X117" s="21">
-        <f>COUNTIF($C$2:$C$271,C117)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10151,7 +10243,7 @@
         <v>103</v>
       </c>
       <c r="X118" s="21">
-        <f>COUNTIF($C$2:$C$271,C118)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10223,7 +10315,7 @@
         <v>98</v>
       </c>
       <c r="X119" s="21">
-        <f>COUNTIF($C$2:$C$271,C119)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10295,7 +10387,7 @@
         <v>105</v>
       </c>
       <c r="X120" s="21">
-        <f>COUNTIF($C$2:$C$271,C120)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10367,7 +10459,7 @@
         <v>105</v>
       </c>
       <c r="X121" s="21">
-        <f>COUNTIF($C$2:$C$271,C121)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10439,7 +10531,7 @@
         <v>100</v>
       </c>
       <c r="X122" s="21">
-        <f>COUNTIF($C$2:$C$271,C122)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10511,7 +10603,7 @@
         <v>100</v>
       </c>
       <c r="X123" s="21">
-        <f>COUNTIF($C$2:$C$271,C123)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10583,7 +10675,7 @@
         <v>100</v>
       </c>
       <c r="X124" s="21">
-        <f>COUNTIF($C$2:$C$271,C124)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10655,7 +10747,7 @@
         <v>101</v>
       </c>
       <c r="X125" s="21">
-        <f>COUNTIF($C$2:$C$271,C125)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10727,7 +10819,7 @@
         <v>103</v>
       </c>
       <c r="X126" s="21">
-        <f>COUNTIF($C$2:$C$271,C126)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10799,7 +10891,7 @@
         <v>100</v>
       </c>
       <c r="X127" s="21">
-        <f>COUNTIF($C$2:$C$271,C127)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -10871,7 +10963,7 @@
         <v>98</v>
       </c>
       <c r="X128" s="21">
-        <f>COUNTIF($C$2:$C$271,C128)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -10943,7 +11035,7 @@
         <v>102</v>
       </c>
       <c r="X129" s="21">
-        <f>COUNTIF($C$2:$C$271,C129)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -11015,7 +11107,7 @@
         <v>102</v>
       </c>
       <c r="X130" s="21">
-        <f>COUNTIF($C$2:$C$271,C130)</f>
+        <f t="shared" ref="X130:X193" si="2">COUNTIF($C$2:$C$271,C130)</f>
         <v>1</v>
       </c>
     </row>
@@ -11087,7 +11179,7 @@
         <v>100</v>
       </c>
       <c r="X131" s="21">
-        <f>COUNTIF($C$2:$C$271,C131)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11159,7 +11251,7 @@
         <v>99</v>
       </c>
       <c r="X132" s="21">
-        <f>COUNTIF($C$2:$C$271,C132)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11231,7 +11323,7 @@
         <v>99</v>
       </c>
       <c r="X133" s="21">
-        <f>COUNTIF($C$2:$C$271,C133)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11303,7 +11395,7 @@
         <v>98</v>
       </c>
       <c r="X134" s="21">
-        <f>COUNTIF($C$2:$C$271,C134)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11375,7 +11467,7 @@
         <v>99</v>
       </c>
       <c r="X135" s="21">
-        <f>COUNTIF($C$2:$C$271,C135)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11447,7 +11539,7 @@
         <v>102</v>
       </c>
       <c r="X136" s="21">
-        <f>COUNTIF($C$2:$C$271,C136)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11519,7 +11611,7 @@
         <v>102</v>
       </c>
       <c r="X137" s="21">
-        <f>COUNTIF($C$2:$C$271,C137)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11591,7 +11683,7 @@
         <v>99</v>
       </c>
       <c r="X138" s="21">
-        <f>COUNTIF($C$2:$C$271,C138)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11663,7 +11755,7 @@
         <v>101</v>
       </c>
       <c r="X139" s="21">
-        <f>COUNTIF($C$2:$C$271,C139)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11735,7 +11827,7 @@
         <v>98</v>
       </c>
       <c r="X140" s="21">
-        <f>COUNTIF($C$2:$C$271,C140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11807,7 +11899,7 @@
         <v>104</v>
       </c>
       <c r="X141" s="21">
-        <f>COUNTIF($C$2:$C$271,C141)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11879,7 +11971,7 @@
         <v>103</v>
       </c>
       <c r="X142" s="21">
-        <f>COUNTIF($C$2:$C$271,C142)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11951,7 +12043,7 @@
         <v>100</v>
       </c>
       <c r="X143" s="21">
-        <f>COUNTIF($C$2:$C$271,C143)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12023,7 +12115,7 @@
         <v>98</v>
       </c>
       <c r="X144" s="21">
-        <f>COUNTIF($C$2:$C$271,C144)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12095,7 +12187,7 @@
         <v>100</v>
       </c>
       <c r="X145" s="21">
-        <f>COUNTIF($C$2:$C$271,C145)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12167,7 +12259,7 @@
         <v>99</v>
       </c>
       <c r="X146" s="21">
-        <f>COUNTIF($C$2:$C$271,C146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12239,7 +12331,7 @@
         <v>102</v>
       </c>
       <c r="X147" s="21">
-        <f>COUNTIF($C$2:$C$271,C147)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12311,7 +12403,7 @@
         <v>101</v>
       </c>
       <c r="X148" s="21">
-        <f>COUNTIF($C$2:$C$271,C148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12383,7 +12475,7 @@
         <v>103</v>
       </c>
       <c r="X149" s="21">
-        <f>COUNTIF($C$2:$C$271,C149)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12455,7 +12547,7 @@
         <v>94</v>
       </c>
       <c r="X150" s="21">
-        <f>COUNTIF($C$2:$C$271,C150)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12527,7 +12619,7 @@
         <v>99</v>
       </c>
       <c r="X151" s="21">
-        <f>COUNTIF($C$2:$C$271,C151)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12599,7 +12691,7 @@
         <v>99</v>
       </c>
       <c r="X152" s="21">
-        <f>COUNTIF($C$2:$C$271,C152)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12671,7 +12763,7 @@
         <v>102</v>
       </c>
       <c r="X153" s="21">
-        <f>COUNTIF($C$2:$C$271,C153)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12743,7 +12835,7 @@
         <v>102</v>
       </c>
       <c r="X154" s="21">
-        <f>COUNTIF($C$2:$C$271,C154)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12815,7 +12907,7 @@
         <v>108</v>
       </c>
       <c r="X155" s="21">
-        <f>COUNTIF($C$2:$C$271,C155)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12887,7 +12979,7 @@
         <v>100</v>
       </c>
       <c r="X156" s="21">
-        <f>COUNTIF($C$2:$C$271,C156)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -12959,7 +13051,7 @@
         <v>100</v>
       </c>
       <c r="X157" s="21">
-        <f>COUNTIF($C$2:$C$271,C157)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13031,7 +13123,7 @@
         <v>100</v>
       </c>
       <c r="X158" s="21">
-        <f>COUNTIF($C$2:$C$271,C158)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13103,7 +13195,7 @@
         <v>101</v>
       </c>
       <c r="X159" s="21">
-        <f>COUNTIF($C$2:$C$271,C159)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -13175,7 +13267,7 @@
         <v>100</v>
       </c>
       <c r="X160" s="21">
-        <f>COUNTIF($C$2:$C$271,C160)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13247,7 +13339,7 @@
         <v>98</v>
       </c>
       <c r="X161" s="21">
-        <f>COUNTIF($C$2:$C$271,C161)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13319,7 +13411,7 @@
         <v>103</v>
       </c>
       <c r="X162" s="21">
-        <f>COUNTIF($C$2:$C$271,C162)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13391,7 +13483,7 @@
         <v>103</v>
       </c>
       <c r="X163" s="21">
-        <f>COUNTIF($C$2:$C$271,C163)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13463,7 +13555,7 @@
         <v>102</v>
       </c>
       <c r="X164" s="21">
-        <f>COUNTIF($C$2:$C$271,C164)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13535,7 +13627,7 @@
         <v>101</v>
       </c>
       <c r="X165" s="21">
-        <f>COUNTIF($C$2:$C$271,C165)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13607,7 +13699,7 @@
         <v>98</v>
       </c>
       <c r="X166" s="21">
-        <f>COUNTIF($C$2:$C$271,C166)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13679,7 +13771,7 @@
         <v>103</v>
       </c>
       <c r="X167" s="21">
-        <f>COUNTIF($C$2:$C$271,C167)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13751,7 +13843,7 @@
         <v>94</v>
       </c>
       <c r="X168" s="21">
-        <f>COUNTIF($C$2:$C$271,C168)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13823,7 +13915,7 @@
         <v>99</v>
       </c>
       <c r="X169" s="21">
-        <f>COUNTIF($C$2:$C$271,C169)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13895,7 +13987,7 @@
         <v>100</v>
       </c>
       <c r="X170" s="21">
-        <f>COUNTIF($C$2:$C$271,C170)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -13967,7 +14059,7 @@
         <v>106</v>
       </c>
       <c r="X171" s="21">
-        <f>COUNTIF($C$2:$C$271,C171)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14039,7 +14131,7 @@
         <v>101</v>
       </c>
       <c r="X172" s="21">
-        <f>COUNTIF($C$2:$C$271,C172)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14111,7 +14203,7 @@
         <v>99</v>
       </c>
       <c r="X173" s="21">
-        <f>COUNTIF($C$2:$C$271,C173)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14183,7 +14275,7 @@
         <v>99</v>
       </c>
       <c r="X174" s="21">
-        <f>COUNTIF($C$2:$C$271,C174)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14255,7 +14347,7 @@
         <v>98</v>
       </c>
       <c r="X175" s="21">
-        <f>COUNTIF($C$2:$C$271,C175)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14327,7 +14419,7 @@
         <v>98</v>
       </c>
       <c r="X176" s="21">
-        <f>COUNTIF($C$2:$C$271,C176)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14399,7 +14491,7 @@
         <v>100</v>
       </c>
       <c r="X177" s="21">
-        <f>COUNTIF($C$2:$C$271,C177)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14471,7 +14563,7 @@
         <v>98</v>
       </c>
       <c r="X178" s="21">
-        <f>COUNTIF($C$2:$C$271,C178)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14543,7 +14635,7 @@
         <v>102</v>
       </c>
       <c r="X179" s="21">
-        <f>COUNTIF($C$2:$C$271,C179)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14615,7 +14707,7 @@
         <v>98</v>
       </c>
       <c r="X180" s="21">
-        <f>COUNTIF($C$2:$C$271,C180)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14687,7 +14779,7 @@
         <v>97</v>
       </c>
       <c r="X181" s="21">
-        <f>COUNTIF($C$2:$C$271,C181)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14759,7 +14851,7 @@
         <v>100</v>
       </c>
       <c r="X182" s="21">
-        <f>COUNTIF($C$2:$C$271,C182)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -14831,7 +14923,7 @@
         <v>98</v>
       </c>
       <c r="X183" s="21">
-        <f>COUNTIF($C$2:$C$271,C183)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -14903,7 +14995,7 @@
         <v>108</v>
       </c>
       <c r="X184" s="21">
-        <f>COUNTIF($C$2:$C$271,C184)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14975,7 +15067,7 @@
         <v>102</v>
       </c>
       <c r="X185" s="21">
-        <f>COUNTIF($C$2:$C$271,C185)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15047,7 +15139,7 @@
         <v>98</v>
       </c>
       <c r="X186" s="21">
-        <f>COUNTIF($C$2:$C$271,C186)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15119,7 +15211,7 @@
         <v>106</v>
       </c>
       <c r="X187" s="21">
-        <f>COUNTIF($C$2:$C$271,C187)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15191,7 +15283,7 @@
         <v>96</v>
       </c>
       <c r="X188" s="21">
-        <f>COUNTIF($C$2:$C$271,C188)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15263,7 +15355,7 @@
         <v>102</v>
       </c>
       <c r="X189" s="21">
-        <f>COUNTIF($C$2:$C$271,C189)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15335,7 +15427,7 @@
         <v>99</v>
       </c>
       <c r="X190" s="21">
-        <f>COUNTIF($C$2:$C$271,C190)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15407,7 +15499,7 @@
         <v>98</v>
       </c>
       <c r="X191" s="21">
-        <f>COUNTIF($C$2:$C$271,C191)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15479,7 +15571,7 @@
         <v>109</v>
       </c>
       <c r="X192" s="21">
-        <f>COUNTIF($C$2:$C$271,C192)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15551,7 +15643,7 @@
         <v>103</v>
       </c>
       <c r="X193" s="21">
-        <f>COUNTIF($C$2:$C$271,C193)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -15623,7 +15715,7 @@
         <v>96</v>
       </c>
       <c r="X194" s="21">
-        <f>COUNTIF($C$2:$C$271,C194)</f>
+        <f t="shared" ref="X194:X257" si="3">COUNTIF($C$2:$C$271,C194)</f>
         <v>1</v>
       </c>
     </row>
@@ -15695,7 +15787,7 @@
         <v>101</v>
       </c>
       <c r="X195" s="21">
-        <f>COUNTIF($C$2:$C$271,C195)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -15767,7 +15859,7 @@
         <v>97</v>
       </c>
       <c r="X196" s="21">
-        <f>COUNTIF($C$2:$C$271,C196)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -15839,7 +15931,7 @@
         <v>97</v>
       </c>
       <c r="X197" s="21">
-        <f>COUNTIF($C$2:$C$271,C197)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -15911,7 +16003,7 @@
         <v>101</v>
       </c>
       <c r="X198" s="21">
-        <f>COUNTIF($C$2:$C$271,C198)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -15983,7 +16075,7 @@
         <v>98</v>
       </c>
       <c r="X199" s="21">
-        <f>COUNTIF($C$2:$C$271,C199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16055,7 +16147,7 @@
         <v>97</v>
       </c>
       <c r="X200" s="21">
-        <f>COUNTIF($C$2:$C$271,C200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16130,7 +16222,7 @@
         <v>328</v>
       </c>
       <c r="X201" s="21">
-        <f>COUNTIF($C$2:$C$271,C201)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16202,7 +16294,7 @@
         <v>98</v>
       </c>
       <c r="X202" s="21">
-        <f>COUNTIF($C$2:$C$271,C202)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16274,7 +16366,7 @@
         <v>104</v>
       </c>
       <c r="X203" s="21">
-        <f>COUNTIF($C$2:$C$271,C203)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16346,7 +16438,7 @@
         <v>100</v>
       </c>
       <c r="X204" s="21">
-        <f>COUNTIF($C$2:$C$271,C204)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16418,7 +16510,7 @@
         <v>101</v>
       </c>
       <c r="X205" s="21">
-        <f>COUNTIF($C$2:$C$271,C205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16490,7 +16582,7 @@
         <v>97</v>
       </c>
       <c r="X206" s="21">
-        <f>COUNTIF($C$2:$C$271,C206)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16562,7 +16654,7 @@
         <v>104</v>
       </c>
       <c r="X207" s="21">
-        <f>COUNTIF($C$2:$C$271,C207)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16634,7 +16726,7 @@
         <v>98</v>
       </c>
       <c r="X208" s="21">
-        <f>COUNTIF($C$2:$C$271,C208)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16706,7 +16798,7 @@
         <v>105</v>
       </c>
       <c r="X209" s="21">
-        <f>COUNTIF($C$2:$C$271,C209)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16778,7 +16870,7 @@
         <v>100</v>
       </c>
       <c r="X210" s="21">
-        <f>COUNTIF($C$2:$C$271,C210)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16850,7 +16942,7 @@
         <v>98</v>
       </c>
       <c r="X211" s="21">
-        <f>COUNTIF($C$2:$C$271,C211)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16922,7 +17014,7 @@
         <v>97</v>
       </c>
       <c r="X212" s="21">
-        <f>COUNTIF($C$2:$C$271,C212)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -16994,7 +17086,7 @@
         <v>96</v>
       </c>
       <c r="X213" s="21">
-        <f>COUNTIF($C$2:$C$271,C213)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17066,7 +17158,7 @@
         <v>100</v>
       </c>
       <c r="X214" s="21">
-        <f>COUNTIF($C$2:$C$271,C214)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17138,7 +17230,7 @@
         <v>96</v>
       </c>
       <c r="X215" s="21">
-        <f>COUNTIF($C$2:$C$271,C215)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17210,7 +17302,7 @@
         <v>102</v>
       </c>
       <c r="X216" s="21">
-        <f>COUNTIF($C$2:$C$271,C216)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17282,7 +17374,7 @@
         <v>100</v>
       </c>
       <c r="X217" s="21">
-        <f>COUNTIF($C$2:$C$271,C217)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17354,7 +17446,7 @@
         <v>102</v>
       </c>
       <c r="X218" s="21">
-        <f>COUNTIF($C$2:$C$271,C218)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17426,7 +17518,7 @@
         <v>98</v>
       </c>
       <c r="X219" s="21">
-        <f>COUNTIF($C$2:$C$271,C219)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17498,7 +17590,7 @@
         <v>98</v>
       </c>
       <c r="X220" s="21">
-        <f>COUNTIF($C$2:$C$271,C220)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17570,7 +17662,7 @@
         <v>102</v>
       </c>
       <c r="X221" s="21">
-        <f>COUNTIF($C$2:$C$271,C221)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17642,7 +17734,7 @@
         <v>98</v>
       </c>
       <c r="X222" s="21">
-        <f>COUNTIF($C$2:$C$271,C222)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17714,7 +17806,7 @@
         <v>98</v>
       </c>
       <c r="X223" s="21">
-        <f>COUNTIF($C$2:$C$271,C223)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17786,7 +17878,7 @@
         <v>98</v>
       </c>
       <c r="X224" s="21">
-        <f>COUNTIF($C$2:$C$271,C224)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17858,7 +17950,7 @@
         <v>95</v>
       </c>
       <c r="X225" s="21">
-        <f>COUNTIF($C$2:$C$271,C225)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -17930,7 +18022,7 @@
         <v>100</v>
       </c>
       <c r="X226" s="21">
-        <f>COUNTIF($C$2:$C$271,C226)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18002,7 +18094,7 @@
         <v>100</v>
       </c>
       <c r="X227" s="21">
-        <f>COUNTIF($C$2:$C$271,C227)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18077,7 +18169,7 @@
         <v>110</v>
       </c>
       <c r="X228" s="21">
-        <f>COUNTIF($C$2:$C$271,C228)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Y228" s="17"/>
@@ -18150,7 +18242,7 @@
         <v>102</v>
       </c>
       <c r="X229" s="21">
-        <f>COUNTIF($C$2:$C$271,C229)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18222,7 +18314,7 @@
         <v>98</v>
       </c>
       <c r="X230" s="21">
-        <f>COUNTIF($C$2:$C$271,C230)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18294,7 +18386,7 @@
         <v>103</v>
       </c>
       <c r="X231" s="21">
-        <f>COUNTIF($C$2:$C$271,C231)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18366,7 +18458,7 @@
         <v>100</v>
       </c>
       <c r="X232" s="21">
-        <f>COUNTIF($C$2:$C$271,C232)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18438,7 +18530,7 @@
         <v>105</v>
       </c>
       <c r="X233" s="21">
-        <f>COUNTIF($C$2:$C$271,C233)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18510,7 +18602,7 @@
         <v>98</v>
       </c>
       <c r="X234" s="21">
-        <f>COUNTIF($C$2:$C$271,C234)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18582,7 +18674,7 @@
         <v>108</v>
       </c>
       <c r="X235" s="21">
-        <f>COUNTIF($C$2:$C$271,C235)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18657,7 +18749,7 @@
         <v>321</v>
       </c>
       <c r="X236" s="21">
-        <f>COUNTIF($C$2:$C$271,C236)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18732,7 +18824,7 @@
         <v>322</v>
       </c>
       <c r="X237" s="21">
-        <f>COUNTIF($C$2:$C$271,C237)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18807,7 +18899,7 @@
         <v>324</v>
       </c>
       <c r="X238" s="21">
-        <f>COUNTIF($C$2:$C$271,C238)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18882,7 +18974,7 @@
         <v>326</v>
       </c>
       <c r="X239" s="21">
-        <f>COUNTIF($C$2:$C$271,C239)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -18954,7 +19046,7 @@
         <v>104</v>
       </c>
       <c r="X240" s="21">
-        <f>COUNTIF($C$2:$C$271,C240)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19026,7 +19118,7 @@
         <v>103</v>
       </c>
       <c r="X241" s="21">
-        <f>COUNTIF($C$2:$C$271,C241)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19098,7 +19190,7 @@
         <v>99</v>
       </c>
       <c r="X242" s="21">
-        <f>COUNTIF($C$2:$C$271,C242)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19170,7 +19262,7 @@
         <v>100</v>
       </c>
       <c r="X243" s="21">
-        <f>COUNTIF($C$2:$C$271,C243)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19242,7 +19334,7 @@
         <v>102</v>
       </c>
       <c r="X244" s="21">
-        <f>COUNTIF($C$2:$C$271,C244)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19314,7 +19406,7 @@
         <v>98</v>
       </c>
       <c r="X245" s="21">
-        <f>COUNTIF($C$2:$C$271,C245)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19386,7 +19478,7 @@
         <v>100</v>
       </c>
       <c r="X246" s="21">
-        <f>COUNTIF($C$2:$C$271,C246)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19458,7 +19550,7 @@
         <v>48</v>
       </c>
       <c r="X247" s="21">
-        <f>COUNTIF($C$2:$C$271,C247)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19530,7 +19622,7 @@
         <v>103</v>
       </c>
       <c r="X248" s="21">
-        <f>COUNTIF($C$2:$C$271,C248)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19602,7 +19694,7 @@
         <v>104</v>
       </c>
       <c r="X249" s="21">
-        <f>COUNTIF($C$2:$C$271,C249)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19674,7 +19766,7 @@
         <v>99</v>
       </c>
       <c r="X250" s="21">
-        <f>COUNTIF($C$2:$C$271,C250)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19746,7 +19838,7 @@
         <v>104</v>
       </c>
       <c r="X251" s="21">
-        <f>COUNTIF($C$2:$C$271,C251)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19818,7 +19910,7 @@
         <v>103</v>
       </c>
       <c r="X252" s="21">
-        <f>COUNTIF($C$2:$C$271,C252)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19893,7 +19985,7 @@
         <v>288</v>
       </c>
       <c r="X253" s="21">
-        <f>COUNTIF($C$2:$C$271,C253)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19968,7 +20060,7 @@
         <v>290</v>
       </c>
       <c r="X254" s="21">
-        <f>COUNTIF($C$2:$C$271,C254)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20043,7 +20135,7 @@
         <v>291</v>
       </c>
       <c r="X255" s="21">
-        <f>COUNTIF($C$2:$C$271,C255)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20118,7 +20210,7 @@
         <v>294</v>
       </c>
       <c r="X256" s="21">
-        <f>COUNTIF($C$2:$C$271,C256)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20193,7 +20285,7 @@
         <v>295</v>
       </c>
       <c r="X257" s="21">
-        <f>COUNTIF($C$2:$C$271,C257)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20268,7 +20360,7 @@
         <v>298</v>
       </c>
       <c r="X258" s="21">
-        <f>COUNTIF($C$2:$C$271,C258)</f>
+        <f t="shared" ref="X258:X271" si="4">COUNTIF($C$2:$C$271,C258)</f>
         <v>1</v>
       </c>
     </row>
@@ -20343,7 +20435,7 @@
         <v>299</v>
       </c>
       <c r="X259" s="21">
-        <f>COUNTIF($C$2:$C$271,C259)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20418,7 +20510,7 @@
         <v>300</v>
       </c>
       <c r="X260" s="21">
-        <f>COUNTIF($C$2:$C$271,C260)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20493,7 +20585,7 @@
         <v>301</v>
       </c>
       <c r="X261" s="21">
-        <f>COUNTIF($C$2:$C$271,C261)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20568,7 +20660,7 @@
         <v>304</v>
       </c>
       <c r="X262" s="21">
-        <f>COUNTIF($C$2:$C$271,C262)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20643,7 +20735,7 @@
         <v>306</v>
       </c>
       <c r="X263" s="21">
-        <f>COUNTIF($C$2:$C$271,C263)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20718,7 +20810,7 @@
         <v>308</v>
       </c>
       <c r="X264" s="21">
-        <f>COUNTIF($C$2:$C$271,C264)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20793,7 +20885,7 @@
         <v>310</v>
       </c>
       <c r="X265" s="21">
-        <f>COUNTIF($C$2:$C$271,C265)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20868,7 +20960,7 @@
         <v>311</v>
       </c>
       <c r="X266" s="21">
-        <f>COUNTIF($C$2:$C$271,C266)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -20943,7 +21035,7 @@
         <v>313</v>
       </c>
       <c r="X267" s="21">
-        <f>COUNTIF($C$2:$C$271,C267)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -21018,7 +21110,7 @@
         <v>314</v>
       </c>
       <c r="X268" s="21">
-        <f>COUNTIF($C$2:$C$271,C268)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -21093,7 +21185,7 @@
         <v>315</v>
       </c>
       <c r="X269" s="21">
-        <f>COUNTIF($C$2:$C$271,C269)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -21168,7 +21260,7 @@
         <v>316</v>
       </c>
       <c r="X270" s="21">
-        <f>COUNTIF($C$2:$C$271,C270)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -21243,7 +21335,7 @@
         <v>319</v>
       </c>
       <c r="X271" s="16">
-        <f>COUNTIF($C$2:$C$271,C271)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -22634,7 +22726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O487"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
@@ -40458,4 +40550,227 @@
     <oddFooter>&amp;C&amp;"Arial,Bold"&amp;9&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECF1245-4C24-4273-98A1-236AD8AF9A5A}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="33">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="33">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" s="33">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="33">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C6" s="33">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="33">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="33">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" s="33">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="33">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>340</v>
+      </c>
+      <c r="C11" s="33">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>341</v>
+      </c>
+      <c r="C12" s="33">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C13" s="33">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="33">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f>SUM(C2:C14)</f>
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>